<commit_message>
Add pwm.c to keil project, add AF_PIN_TYPE_PWM_PWMxx enums to pin_defs_mcu.h
</commit_message>
<xml_diff>
--- a/docs/信号定义.xlsx
+++ b/docs/信号定义.xlsx
@@ -824,23 +824,28 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>21124</xdr:colOff>
+      <xdr:colOff>8282</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>178318</xdr:rowOff>
+      <xdr:rowOff>173935</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2609847" cy="3296236"/>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>7453</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>40585</xdr:rowOff>
+    </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPr id="4" name="图片 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -854,8 +859,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3069124" y="178318"/>
-          <a:ext cx="2609847" cy="3296236"/>
+          <a:off x="4422912" y="364435"/>
+          <a:ext cx="2616476" cy="3295650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -873,29 +878,29 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>2074</xdr:colOff>
+      <xdr:colOff>8283</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>159268</xdr:rowOff>
+      <xdr:rowOff>165658</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>8665</xdr:colOff>
+      <xdr:colOff>15737</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>26504</xdr:rowOff>
+      <xdr:rowOff>32308</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="图片 2"/>
+        <xdr:cNvPr id="5" name="图片 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -909,8 +914,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="13413274" y="159268"/>
-          <a:ext cx="2609847" cy="3296236"/>
+          <a:off x="16209066" y="356158"/>
+          <a:ext cx="2616476" cy="3295650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1720,20 +1725,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:AL24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" customWidth="1"/>
     <col min="10" max="10" width="3" customWidth="1"/>
     <col min="11" max="11" width="7.5703125" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" customWidth="1"/>
     <col min="18" max="18" width="10.140625" customWidth="1"/>
-    <col min="19" max="19" width="9.42578125" customWidth="1"/>
+    <col min="19" max="19" width="6.28515625" customWidth="1"/>
     <col min="20" max="20" width="16.85546875" customWidth="1"/>
     <col min="21" max="21" width="12.28515625" customWidth="1"/>
     <col min="22" max="22" width="13.7109375" customWidth="1"/>

</xml_diff>

<commit_message>
bugfix: if 'main.py' is running when executing another script from OpenMV IDE, fb alloc buffer may fail, fixed by soft reset when staring a new script in OpenMV IDE, the cost is user have to press start button twice to start it. upgrade all upgradable OpenMV firmware to 3.3.1
</commit_message>
<xml_diff>
--- a/docs/信号定义.xlsx
+++ b/docs/信号定义.xlsx
@@ -643,7 +643,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -662,7 +662,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1090,8 +1089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AM24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AL19" sqref="AL19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1488,11 +1487,11 @@
       <c r="AK11" s="1"/>
     </row>
     <row r="12" spans="2:39">
-      <c r="C12" s="17"/>
-      <c r="D12" s="18" t="s">
+      <c r="C12" s="16"/>
+      <c r="D12" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="28" t="s">
         <v>82</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -1519,7 +1518,7 @@
       <c r="W12" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="X12" s="30" t="s">
+      <c r="X12" s="29" t="s">
         <v>96</v>
       </c>
       <c r="Y12" s="2" t="s">
@@ -1542,14 +1541,14 @@
         <v>38</v>
       </c>
       <c r="AJ12" s="1"/>
-      <c r="AK12" s="1"/>
+      <c r="AK12" s="18"/>
     </row>
     <row r="13" spans="2:39">
-      <c r="C13" s="17"/>
-      <c r="D13" s="18" t="s">
+      <c r="C13" s="16"/>
+      <c r="D13" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="28" t="s">
         <v>83</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -1572,22 +1571,22 @@
       <c r="O13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P13" s="22" t="s">
+      <c r="P13" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="Q13" s="24" t="s">
+      <c r="Q13" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="R13" s="18" t="s">
+      <c r="R13" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="S13" s="21" t="s">
+      <c r="S13" s="20" t="s">
         <v>63</v>
       </c>
       <c r="W13" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="X13" s="30" t="s">
+      <c r="X13" s="29" t="s">
         <v>97</v>
       </c>
       <c r="Y13" s="2" t="s">
@@ -1613,22 +1612,22 @@
       <c r="AI13" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AJ13" s="24" t="s">
+      <c r="AJ13" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="AK13" s="13" t="s">
+      <c r="AK13" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="AL13" s="15" t="s">
+      <c r="AL13" s="20" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="14" spans="2:39">
-      <c r="C14" s="17"/>
-      <c r="D14" s="18" t="s">
+      <c r="C14" s="16"/>
+      <c r="D14" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="28" t="s">
         <v>87</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -1647,16 +1646,16 @@
       <c r="M14" s="1"/>
       <c r="N14" s="5"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="25" t="s">
+      <c r="P14" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="19"/>
-      <c r="S14" s="17"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="16"/>
       <c r="W14" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="X14" s="30" t="s">
+      <c r="X14" s="29" t="s">
         <v>98</v>
       </c>
       <c r="Y14" s="2" t="s">
@@ -1678,14 +1677,14 @@
       <c r="AI14" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="AK14" s="1"/>
+      <c r="AK14" s="18"/>
     </row>
     <row r="15" spans="2:39">
-      <c r="C15" s="17"/>
-      <c r="D15" s="18" t="s">
+      <c r="C15" s="16"/>
+      <c r="D15" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="28" t="s">
         <v>84</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -1708,22 +1707,22 @@
       <c r="O15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P15" s="22" t="s">
+      <c r="P15" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="Q15" s="24" t="s">
+      <c r="Q15" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="R15" s="18" t="s">
+      <c r="R15" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="S15" s="21" t="s">
+      <c r="S15" s="20" t="s">
         <v>64</v>
       </c>
       <c r="W15" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="X15" s="30" t="s">
+      <c r="X15" s="29" t="s">
         <v>99</v>
       </c>
       <c r="Y15" s="2" t="s">
@@ -1749,10 +1748,10 @@
       <c r="AI15" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AJ15" s="24" t="s">
+      <c r="AJ15" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="AK15" s="13" t="s">
+      <c r="AK15" s="22" t="s">
         <v>90</v>
       </c>
       <c r="AL15" s="15" t="s">
@@ -1760,11 +1759,11 @@
       </c>
     </row>
     <row r="16" spans="2:39">
-      <c r="C16" s="17"/>
-      <c r="D16" s="20" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="28" t="s">
         <v>85</v>
       </c>
       <c r="F16" s="6" t="s">
@@ -1787,25 +1786,25 @@
       <c r="O16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P16" s="22" t="s">
+      <c r="P16" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="Q16" s="26" t="s">
+      <c r="Q16" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="R16" s="23" t="s">
+      <c r="R16" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="S16" s="21" t="s">
+      <c r="S16" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="T16" s="28" t="s">
+      <c r="T16" s="27" t="s">
         <v>79</v>
       </c>
       <c r="W16" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="X16" s="30" t="s">
+      <c r="X16" s="29" t="s">
         <v>100</v>
       </c>
       <c r="Y16" s="6" t="s">
@@ -1834,27 +1833,27 @@
       <c r="AJ16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AK16" s="13" t="s">
+      <c r="AK16" s="22" t="s">
         <v>89</v>
       </c>
       <c r="AL16" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="AM16" s="16" t="s">
+      <c r="AM16" s="27" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="17" spans="2:39">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="28" t="s">
         <v>86</v>
       </c>
       <c r="F17" s="6" t="s">
@@ -1877,19 +1876,19 @@
       <c r="O17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P17" s="22" t="s">
+      <c r="P17" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="Q17" s="26" t="s">
+      <c r="Q17" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="R17" s="23" t="s">
+      <c r="R17" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="S17" s="21" t="s">
+      <c r="S17" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="T17" s="28" t="s">
+      <c r="T17" s="27" t="s">
         <v>68</v>
       </c>
       <c r="U17" s="15" t="s">
@@ -1901,7 +1900,7 @@
       <c r="W17" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="X17" s="30" t="s">
+      <c r="X17" s="29" t="s">
         <v>101</v>
       </c>
       <c r="Y17" s="6" t="s">
@@ -1930,13 +1929,13 @@
       <c r="AJ17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AK17" s="13" t="s">
+      <c r="AK17" s="22" t="s">
         <v>88</v>
       </c>
       <c r="AL17" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="AM17" s="16" t="s">
+      <c r="AM17" s="27" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2052,7 +2051,7 @@
       </c>
     </row>
     <row r="24" spans="2:39">
-      <c r="X24" s="27" t="s">
+      <c r="X24" s="26" t="s">
         <v>102</v>
       </c>
     </row>

</xml_diff>